<commit_message>
Add minimal formatting to Excel sheet
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
@@ -569,6 +569,63 @@
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B32" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:B32"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="keyword"/>
+    <tableColumn id="2" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I5" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I5"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="position"/>
+    <tableColumn id="2" name="variable"/>
+    <tableColumn id="3" name="type"/>
+    <tableColumn id="4" name="en_long_name"/>
+    <tableColumn id="5" name="fo_long_name"/>
+    <tableColumn id="6" name="en_elimination"/>
+    <tableColumn id="7" name="fo_elimination"/>
+    <tableColumn id="8" name="en_note"/>
+    <tableColumn id="9" name="fo_note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F11" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="variable"/>
+    <tableColumn id="2" name="code"/>
+    <tableColumn id="3" name="sortorder"/>
+    <tableColumn id="4" name="en_code_label"/>
+    <tableColumn id="5" name="fo_code_label"/>
+    <tableColumn id="6" name="precision"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D85" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D85"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="event"/>
+    <tableColumn id="2" name="gender"/>
+    <tableColumn id="3" name="time"/>
+    <tableColumn id="4" name=".figures"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,9 +909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="44.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1115,6 +1176,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1122,9 +1186,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="7.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="17.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="26.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="29.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="32.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="32.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1244,6 +1319,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1251,9 +1329,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="9.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="26.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="35.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="9.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1458,6 +1544,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1465,9 +1554,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="5.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="6.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="6.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -2662,5 +2757,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rename .figures to figures_ in metadata
Close #104
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
@@ -197,7 +197,7 @@
     <t xml:space="preserve">time</t>
   </si>
   <si>
-    <t xml:space="preserve">.figures</t>
+    <t xml:space="preserve">figures_</t>
   </si>
   <si>
     <t xml:space="preserve">figures</t>
@@ -519,7 +519,7 @@
     <tableColumn id="1" name="til- og frágongd"/>
     <tableColumn id="2" name="køn"/>
     <tableColumn id="3" name="tid"/>
-    <tableColumn id="4" name=".figures"/>
+    <tableColumn id="4" name="figures_"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Break lines longer than 256 characthers
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">keyword</t>
   </si>
@@ -38,15 +38,12 @@
     <t xml:space="preserve">LANGUAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">en</t>
+    <t xml:space="preserve">fo</t>
   </si>
   <si>
     <t xml:space="preserve">LANGUAGES</t>
   </si>
   <si>
-    <t xml:space="preserve">en","fo</t>
-  </si>
-  <si>
     <t xml:space="preserve">CREATION-DATE</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t xml:space="preserve">BE</t>
   </si>
   <si>
-    <t xml:space="preserve">SUBJECT-AREA_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population</t>
-  </si>
-  <si>
     <t xml:space="preserve">SUBJECT-AREA_fo</t>
   </si>
   <si>
@@ -104,102 +95,60 @@
     <t xml:space="preserve">YES</t>
   </si>
   <si>
-    <t xml:space="preserve">DESCRIPTION_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTPopulation January 1st 2018-2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">DESCRIPTION_fo</t>
   </si>
   <si>
     <t xml:space="preserve">TESTBefolkningen pr 1. januar 2018 - 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTENTS_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population January 1st</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONTENTS_fo</t>
   </si>
   <si>
     <t xml:space="preserve">Befolkningen 1. januar</t>
   </si>
   <si>
-    <t xml:space="preserve">UNITS_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">persons</t>
-  </si>
-  <si>
     <t xml:space="preserve">UNITS_fo</t>
   </si>
   <si>
     <t xml:space="preserve">personer</t>
   </si>
   <si>
-    <t xml:space="preserve">LAST-UPDATED_en</t>
+    <t xml:space="preserve">LAST-UPDATED_fo</t>
   </si>
   <si>
     <t xml:space="preserve">20210211 09:00</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTACT_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lars Pedersen, LARP@stat.gl</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONTACT_fo</t>
   </si>
   <si>
     <t xml:space="preserve">test, Lars Pedersen, LARP@stat.gl</t>
   </si>
   <si>
-    <t xml:space="preserve">SOURCE_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics Greenland</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOURCE_fo</t>
   </si>
   <si>
     <t xml:space="preserve">Grønlands Statistik</t>
   </si>
   <si>
-    <t xml:space="preserve">LINK_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.stat.gl/bee202201/m1</t>
-  </si>
-  <si>
     <t xml:space="preserve">LINK_fo</t>
   </si>
   <si>
     <t xml:space="preserve">www.stat.gl/bed202201/m1</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTEX_en</t>
+    <t xml:space="preserve">NOTEX_fo</t>
   </si>
   <si>
     <t xml:space="preserve">Tvungen fodnote</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTEX_fo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE_en</t>
+    <t xml:space="preserve">NOTE_fo</t>
   </si>
   <si>
     <t xml:space="preserve">Befolkningsstatistikregistret indeholder …</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE_fo</t>
-  </si>
-  <si>
     <t xml:space="preserve">position</t>
   </si>
   <si>
@@ -209,36 +158,21 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">en_long_name</t>
-  </si>
-  <si>
     <t xml:space="preserve">fo_long_name</t>
   </si>
   <si>
-    <t xml:space="preserve">en_elimination</t>
-  </si>
-  <si>
     <t xml:space="preserve">fo_elimination</t>
   </si>
   <si>
-    <t xml:space="preserve">en_note</t>
-  </si>
-  <si>
     <t xml:space="preserve">fo_note</t>
   </si>
   <si>
     <t xml:space="preserve">S1</t>
   </si>
   <si>
-    <t xml:space="preserve">event</t>
-  </si>
-  <si>
     <t xml:space="preserve">til- og frágongd</t>
   </si>
   <si>
-    <t xml:space="preserve">Population (start of year)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fólkatalið fyrst í árinum</t>
   </si>
   <si>
@@ -248,28 +182,22 @@
     <t xml:space="preserve">S2</t>
   </si>
   <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
     <t xml:space="preserve">køn</t>
   </si>
   <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
     <t xml:space="preserve">I alt</t>
   </si>
   <si>
     <t xml:space="preserve">H1</t>
   </si>
   <si>
+    <t xml:space="preserve">tid</t>
+  </si>
+  <si>
     <t xml:space="preserve">time</t>
   </si>
   <si>
-    <t xml:space="preserve">tid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.figures</t>
+    <t xml:space="preserve">figures_</t>
   </si>
   <si>
     <t xml:space="preserve">figures</t>
@@ -281,91 +209,64 @@
     <t xml:space="preserve">sortorder</t>
   </si>
   <si>
-    <t xml:space="preserve">en_code_label</t>
-  </si>
-  <si>
     <t xml:space="preserve">fo_code_label</t>
   </si>
   <si>
     <t xml:space="preserve">precision</t>
   </si>
   <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mænd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kvinder</t>
+  </si>
+  <si>
     <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">Birth</t>
-  </si>
-  <si>
     <t xml:space="preserve">Livandi fødd</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">Immigration</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flutt til Føroya</t>
   </si>
   <si>
     <t xml:space="preserve">O</t>
   </si>
   <si>
-    <t xml:space="preserve">Emigration</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flutt úr Føroyum</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">Death</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deyð</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">Correction</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rættingar</t>
   </si>
   <si>
     <t xml:space="preserve">U</t>
   </si>
   <si>
-    <t xml:space="preserve">Population (end of year)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fólkatalið síðst í mánaðinum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Men</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mænd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kvinder</t>
   </si>
   <si>
     <t xml:space="preserve">2000Q1</t>
@@ -572,8 +473,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B32" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B23" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:B23"/>
   <tableColumns count="2">
     <tableColumn id="1" name="keyword"/>
     <tableColumn id="2" name="value"/>
@@ -583,33 +484,29 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I5" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I5"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F5" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="position"/>
     <tableColumn id="2" name="variable"/>
     <tableColumn id="3" name="type"/>
-    <tableColumn id="4" name="en_long_name"/>
-    <tableColumn id="5" name="fo_long_name"/>
-    <tableColumn id="6" name="en_elimination"/>
-    <tableColumn id="7" name="fo_elimination"/>
-    <tableColumn id="8" name="en_note"/>
-    <tableColumn id="9" name="fo_note"/>
+    <tableColumn id="4" name="fo_long_name"/>
+    <tableColumn id="5" name="fo_elimination"/>
+    <tableColumn id="6" name="fo_note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F11" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:F11"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E11" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E11"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="variable"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="sortorder"/>
-    <tableColumn id="4" name="en_code_label"/>
-    <tableColumn id="5" name="fo_code_label"/>
-    <tableColumn id="6" name="precision"/>
+    <tableColumn id="4" name="fo_code_label"/>
+    <tableColumn id="5" name="precision"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,10 +516,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D85" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:D85"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="event"/>
-    <tableColumn id="2" name="gender"/>
-    <tableColumn id="3" name="time"/>
-    <tableColumn id="4" name=".figures"/>
+    <tableColumn id="1" name="til- og frágongd"/>
+    <tableColumn id="2" name="køn"/>
+    <tableColumn id="3" name="tid"/>
+    <tableColumn id="4" name="figures_"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -954,223 +851,151 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1191,130 +1016,94 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="17.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="7.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="17.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="26.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="29.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="32.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="32.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="29.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="32.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3"/>
+        <v>56</v>
+      </c>
+      <c r="F3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E4"/>
       <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
     </row>
     <row r="5">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1333,213 +1122,179 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="9.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="26.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="35.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="9.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="35.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="9.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
-        <v>86</v>
-      </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2"/>
+        <v>56</v>
+      </c>
+      <c r="E2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3"/>
+        <v>68</v>
+      </c>
+      <c r="E3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4"/>
+        <v>70</v>
+      </c>
+      <c r="E4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5"/>
+        <v>52</v>
+      </c>
+      <c r="E5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6"/>
+        <v>73</v>
+      </c>
+      <c r="E6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7"/>
+        <v>75</v>
+      </c>
+      <c r="E7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8"/>
+        <v>77</v>
+      </c>
+      <c r="E8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>79</v>
       </c>
-      <c r="E9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9"/>
+      <c r="E9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10"/>
+        <v>81</v>
+      </c>
+      <c r="E10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11"/>
+        <v>83</v>
+      </c>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1558,1200 +1313,1200 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="5.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="6.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="6.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s">
         <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D54" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D55" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D59" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D60" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D68" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D70" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C74" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D74" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C76" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D76" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C78" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D78" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C79" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D79" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C80" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D80" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="D82" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make Excel table theme less dominent
Close #126
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
@@ -479,7 +479,7 @@
     <tableColumn id="1" name="keyword"/>
     <tableColumn id="2" name="value"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -494,7 +494,7 @@
     <tableColumn id="5" name="fo_elimination"/>
     <tableColumn id="6" name="fo_note"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -508,7 +508,7 @@
     <tableColumn id="4" name="fo_code_label"/>
     <tableColumn id="5" name="precision"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -521,7 +521,7 @@
     <tableColumn id="3" name="tid"/>
     <tableColumn id="4" name="figures_"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 

</xml_diff>

<commit_message>
Bugfix: Remove quotes around YES in elimination
Close #118
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_FOTEST_by_metamake.xlsx
@@ -479,7 +479,7 @@
     <tableColumn id="1" name="keyword"/>
     <tableColumn id="2" name="value"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -494,7 +494,7 @@
     <tableColumn id="5" name="fo_elimination"/>
     <tableColumn id="6" name="fo_note"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -508,7 +508,7 @@
     <tableColumn id="4" name="fo_code_label"/>
     <tableColumn id="5" name="precision"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -521,7 +521,7 @@
     <tableColumn id="3" name="tid"/>
     <tableColumn id="4" name="figures_"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 

</xml_diff>